<commit_message>
Finished 5 differents methods
</commit_message>
<xml_diff>
--- a/python/posts/cathet.xlsx
+++ b/python/posts/cathet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\developer\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34CD5F13-6713-49C3-A42B-B61896A33189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61E503C-0889-4250-97A1-D9702DC24D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw" sheetId="1" r:id="rId1"/>
+    <sheet name="Manual" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,6 +96,170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="GraphFull"/>
+      <sheetName val="Graph"/>
+      <sheetName val="GraphFit"/>
+      <sheetName val="Zoom1"/>
+      <sheetName val="Zoom2"/>
+      <sheetName val="Zoom3"/>
+      <sheetName val="&lt;v&gt;"/>
+      <sheetName val="vfit"/>
+      <sheetName val="vT"/>
+      <sheetName val="vTbis"/>
+      <sheetName val="Data"/>
+      <sheetName val="Data2"/>
+      <sheetName val="Data2Bis"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11">
+        <row r="16">
+          <cell r="F16" t="str">
+            <v>v</v>
+          </cell>
+          <cell r="G16" t="str">
+            <v>t</v>
+          </cell>
+          <cell r="H16" t="str">
+            <v>bP/bR</v>
+          </cell>
+          <cell r="I16" t="str">
+            <v>1/v</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="F17">
+            <v>1.1040935672514621E-5</v>
+          </cell>
+          <cell r="G17">
+            <v>279</v>
+          </cell>
+          <cell r="H17">
+            <v>1.8234723549376672E-3</v>
+          </cell>
+          <cell r="I17">
+            <v>90572.033898305075</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="F18">
+            <v>8.2162162162162168E-6</v>
+          </cell>
+          <cell r="G18">
+            <v>424</v>
+          </cell>
+          <cell r="H18">
+            <v>2.3521926394042482E-3</v>
+          </cell>
+          <cell r="I18">
+            <v>121710.52631578947</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="F19">
+            <v>7.527426160337553E-6</v>
+          </cell>
+          <cell r="G19">
+            <v>1150</v>
+          </cell>
+          <cell r="H19">
+            <v>4.7313165457712313E-3</v>
+          </cell>
+          <cell r="I19">
+            <v>132847.533632287</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="F20">
+            <v>6.6000000000000003E-6</v>
+          </cell>
+          <cell r="G20">
+            <v>1938</v>
+          </cell>
+          <cell r="H20">
+            <v>7.0245106397895133E-3</v>
+          </cell>
+          <cell r="I20">
+            <v>151515.15151515152</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="F21">
+            <v>6.6461538461538454E-6</v>
+          </cell>
+          <cell r="G21">
+            <v>3218</v>
+          </cell>
+          <cell r="H21">
+            <v>1.0281095703954815E-2</v>
+          </cell>
+          <cell r="I21">
+            <v>150462.96296296298</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="F22">
+            <v>5.1666666666666666E-6</v>
+          </cell>
+          <cell r="G22">
+            <v>4108</v>
+          </cell>
+          <cell r="H22">
+            <v>1.2358446998034369E-2</v>
+          </cell>
+          <cell r="I22">
+            <v>193548.38709677418</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="F23">
+            <v>4.6666666666666663E-6</v>
+          </cell>
+          <cell r="G23">
+            <v>5084</v>
+          </cell>
+          <cell r="H23">
+            <v>1.4324163595185051E-2</v>
+          </cell>
+          <cell r="I23">
+            <v>214285.71428571429</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="F24">
+            <v>4.1968999999999996E-6</v>
+          </cell>
+          <cell r="G24">
+            <v>6908</v>
+          </cell>
+          <cell r="H24">
+            <v>1.7669736536587918E-2</v>
+          </cell>
+          <cell r="I24">
+            <v>238271.10486311329</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="12"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,7 +558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1354,4 +1522,181 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA303683-EF75-4EFB-A02B-1668F64145AE}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f>[1]Data2!F16</f>
+        <v>v</v>
+      </c>
+      <c r="B1" t="str">
+        <f>[1]Data2!G16</f>
+        <v>t</v>
+      </c>
+      <c r="C1" t="str">
+        <f>[1]Data2!H16</f>
+        <v>bP/bR</v>
+      </c>
+      <c r="D1" t="str">
+        <f>[1]Data2!I16</f>
+        <v>1/v</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>[1]Data2!F17</f>
+        <v>1.1040935672514621E-5</v>
+      </c>
+      <c r="B2">
+        <f>[1]Data2!G17</f>
+        <v>279</v>
+      </c>
+      <c r="C2">
+        <f>[1]Data2!H17</f>
+        <v>1.8234723549376672E-3</v>
+      </c>
+      <c r="D2">
+        <f>[1]Data2!I17</f>
+        <v>90572.033898305075</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>[1]Data2!F18</f>
+        <v>8.2162162162162168E-6</v>
+      </c>
+      <c r="B3">
+        <f>[1]Data2!G18</f>
+        <v>424</v>
+      </c>
+      <c r="C3">
+        <f>[1]Data2!H18</f>
+        <v>2.3521926394042482E-3</v>
+      </c>
+      <c r="D3">
+        <f>[1]Data2!I18</f>
+        <v>121710.52631578947</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>[1]Data2!F19</f>
+        <v>7.527426160337553E-6</v>
+      </c>
+      <c r="B4">
+        <f>[1]Data2!G19</f>
+        <v>1150</v>
+      </c>
+      <c r="C4">
+        <f>[1]Data2!H19</f>
+        <v>4.7313165457712313E-3</v>
+      </c>
+      <c r="D4">
+        <f>[1]Data2!I19</f>
+        <v>132847.533632287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>[1]Data2!F20</f>
+        <v>6.6000000000000003E-6</v>
+      </c>
+      <c r="B5">
+        <f>[1]Data2!G20</f>
+        <v>1938</v>
+      </c>
+      <c r="C5">
+        <f>[1]Data2!H20</f>
+        <v>7.0245106397895133E-3</v>
+      </c>
+      <c r="D5">
+        <f>[1]Data2!I20</f>
+        <v>151515.15151515152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>[1]Data2!F21</f>
+        <v>6.6461538461538454E-6</v>
+      </c>
+      <c r="B6">
+        <f>[1]Data2!G21</f>
+        <v>3218</v>
+      </c>
+      <c r="C6">
+        <f>[1]Data2!H21</f>
+        <v>1.0281095703954815E-2</v>
+      </c>
+      <c r="D6">
+        <f>[1]Data2!I21</f>
+        <v>150462.96296296298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f>[1]Data2!F22</f>
+        <v>5.1666666666666666E-6</v>
+      </c>
+      <c r="B7">
+        <f>[1]Data2!G22</f>
+        <v>4108</v>
+      </c>
+      <c r="C7">
+        <f>[1]Data2!H22</f>
+        <v>1.2358446998034369E-2</v>
+      </c>
+      <c r="D7">
+        <f>[1]Data2!I22</f>
+        <v>193548.38709677418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>[1]Data2!F23</f>
+        <v>4.6666666666666663E-6</v>
+      </c>
+      <c r="B8">
+        <f>[1]Data2!G23</f>
+        <v>5084</v>
+      </c>
+      <c r="C8">
+        <f>[1]Data2!H23</f>
+        <v>1.4324163595185051E-2</v>
+      </c>
+      <c r="D8">
+        <f>[1]Data2!I23</f>
+        <v>214285.71428571429</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>[1]Data2!F24</f>
+        <v>4.1968999999999996E-6</v>
+      </c>
+      <c r="B9">
+        <f>[1]Data2!G24</f>
+        <v>6908</v>
+      </c>
+      <c r="C9">
+        <f>[1]Data2!H24</f>
+        <v>1.7669736536587918E-2</v>
+      </c>
+      <c r="D9">
+        <f>[1]Data2!I24</f>
+        <v>238271.10486311329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>